<commit_message>
add generic and case text elements to input xlsx for beerwiser
</commit_message>
<xml_diff>
--- a/src/vlinder/data/beerwiser/xlsx/beerwiser.xlsx
+++ b/src/vlinder/data/beerwiser/xlsx/beerwiser.xlsx
@@ -1,34 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/tRBS/open source/trbs/model/data/beerwiser/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttami001/Documents/forked_tbrs_opensource/trbs/src/vlinder/data/beerwiser/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468B641F-C12C-FB44-9437-884644042C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E66A2B-CD07-B04A-B0AC-690182623AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="-21780" windowWidth="34560" windowHeight="19760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
-    <sheet name="key_outputs" sheetId="2" r:id="rId2"/>
-    <sheet name="decision_makers_options" sheetId="3" r:id="rId3"/>
-    <sheet name="scenarios" sheetId="4" r:id="rId4"/>
-    <sheet name="fixed_inputs" sheetId="5" r:id="rId5"/>
-    <sheet name="dependencies" sheetId="7" r:id="rId6"/>
-    <sheet name="theme_weights" sheetId="8" r:id="rId7"/>
-    <sheet name="key_output_weights" sheetId="9" r:id="rId8"/>
-    <sheet name="scenario_weights" sheetId="10" r:id="rId9"/>
+    <sheet name="generic_text_elements" sheetId="11" r:id="rId2"/>
+    <sheet name="case_text_elements" sheetId="12" r:id="rId3"/>
+    <sheet name="key_outputs" sheetId="2" r:id="rId4"/>
+    <sheet name="decision_makers_options" sheetId="3" r:id="rId5"/>
+    <sheet name="scenarios" sheetId="4" r:id="rId6"/>
+    <sheet name="fixed_inputs" sheetId="5" r:id="rId7"/>
+    <sheet name="dependencies" sheetId="7" r:id="rId8"/>
+    <sheet name="theme_weights" sheetId="8" r:id="rId9"/>
+    <sheet name="key_output_weights" sheetId="9" r:id="rId10"/>
+    <sheet name="scenario_weights" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="84">
   <si>
     <t>configuration</t>
   </si>
@@ -202,15 +204,100 @@
   </si>
   <si>
     <t>squeezed *</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>title_scenarios</t>
+  </si>
+  <si>
+    <t>title_dmo</t>
+  </si>
+  <si>
+    <t>Key outputs</t>
+  </si>
+  <si>
+    <t>title_key_outputs</t>
+  </si>
+  <si>
+    <t>Strategic Challenge</t>
+  </si>
+  <si>
+    <t>title_strategic_challenge</t>
+  </si>
+  <si>
+    <t>generic_text_element</t>
+  </si>
+  <si>
+    <t>strategic_challenge</t>
+  </si>
+  <si>
+    <t>case_text_element</t>
+  </si>
+  <si>
+    <t>text_strategic_challenge</t>
+  </si>
+  <si>
+    <t>title_comparison</t>
+  </si>
+  <si>
+    <t>Comparisons of options</t>
+  </si>
+  <si>
+    <t>title_theme_weights</t>
+  </si>
+  <si>
+    <t>title_scenario_weights</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Describing strategic challenge that requires a decision</t>
+  </si>
+  <si>
+    <t>Which indicators do you use to evaluate the impact of your decision(s)?</t>
+  </si>
+  <si>
+    <t>Which options do you have to influence your impact?</t>
+  </si>
+  <si>
+    <t>Which uncertainty do you want to account for?</t>
+  </si>
+  <si>
+    <t>text_key_outputs</t>
+  </si>
+  <si>
+    <t>text_dmo</t>
+  </si>
+  <si>
+    <t>text_scenarios</t>
+  </si>
+  <si>
+    <t>How to source energy?</t>
+  </si>
+  <si>
+    <t>Key output and theme weights</t>
+  </si>
+  <si>
+    <t>Scenario weights</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -222,13 +309,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -255,17 +355,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{1FD10895-72A3-7148-9AC0-E24F8F49DC8D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -594,7 +701,256 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R36" sqref="R36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897110FD-3CDF-924E-A652-CE81174720E2}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="163.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4671918-A843-C04F-9129-57BE941EA328}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -698,7 +1054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -790,7 +1146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -882,7 +1238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -945,7 +1301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
@@ -1167,7 +1523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1212,98 +1568,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>